<commit_message>
Update driverAthletics Excel files for 2021-2025 with new data
</commit_message>
<xml_diff>
--- a/project/data/driverAthletics2021.xlsx
+++ b/project/data/driverAthletics2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tasna\Documents\Egyetem\dataVizualization\Data-Vizualization\project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912100BF-441F-4515-B94D-F7E80B32D891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13751765-B2B8-4CD4-AA5A-6C8BF0C33A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Lewis Hamilton</t>
   </si>
@@ -142,13 +142,19 @@
   </si>
   <si>
     <t>Age</t>
+  </si>
+  <si>
+    <t>Wins</t>
+  </si>
+  <si>
+    <t>Race Starts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,14 +163,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF1B1C1D"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF1B1C1D"/>
       <name val="Arial"/>
@@ -192,16 +190,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,15 +475,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -501,288 +493,414 @@
       <c r="C1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>73</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="E2" s="1">
+        <v>103</v>
+      </c>
+      <c r="F2" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>69</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="42" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="E3" s="1">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>72</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="E4" s="1">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>63</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>62</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="E6" s="1">
+        <v>53</v>
+      </c>
+      <c r="F6" s="1">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>70</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>68</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="E8" s="1">
+        <v>32</v>
+      </c>
+      <c r="F8" s="1">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>66</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="42" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>66</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="E10" s="1">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>68</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>69</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>64</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>70</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>54</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="42" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>70</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="42" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="E16" s="1">
+        <v>21</v>
+      </c>
+      <c r="F16" s="1">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>75</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>68</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="42" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>67</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>70</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="28" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>73</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>26</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>